<commit_message>
feat: pull 155 companies fin
</commit_message>
<xml_diff>
--- a/data_preparation/scraping/warn-155.xlsx
+++ b/data_preparation/scraping/warn-155.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyler\Desktop\Grad_1B\Big_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf14606d9a4a55b6/sfu/cmpt733/project/cmpt-733-final-project/data_preparation/scraping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2D95D71-B6A3-41D7-8F97-433A08032333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{F2D95D71-B6A3-41D7-8F97-433A08032333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDC6A753-1862-F14E-A146-322A19001524}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{697C4338-14BA-4840-9685-EBB3F77A6725}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33680" windowHeight="19500" xr2:uid="{697C4338-14BA-4840-9685-EBB3F77A6725}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1323,12 +1323,16 @@
   <dimension ref="A1:B156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1336,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1344,7 +1348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1352,7 +1356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1368,7 +1372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1376,7 +1380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1384,7 +1388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1392,7 +1396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1400,7 +1404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1408,7 +1412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1416,7 +1420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1424,7 +1428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1432,7 +1436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1440,7 +1444,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1456,7 +1460,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1464,7 +1468,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1472,7 +1476,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1480,7 +1484,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1496,7 +1500,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1512,7 +1516,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1528,7 +1532,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1536,7 +1540,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1544,7 +1548,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1552,7 +1556,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1560,7 +1564,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1576,7 +1580,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1584,7 +1588,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -1600,7 +1604,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -1608,7 +1612,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1616,7 +1620,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1632,7 +1636,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1640,7 +1644,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1648,7 +1652,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1656,7 +1660,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1664,7 +1668,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -1672,7 +1676,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1680,7 +1684,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1696,7 +1700,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1704,7 +1708,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -1712,7 +1716,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -1720,7 +1724,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -1736,7 +1740,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -1744,7 +1748,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -1752,7 +1756,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -1760,7 +1764,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -1768,7 +1772,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -1776,7 +1780,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -1784,7 +1788,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -1792,7 +1796,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -1800,7 +1804,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -1808,7 +1812,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -1816,7 +1820,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>122</v>
       </c>
@@ -1824,7 +1828,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>126</v>
       </c>
@@ -1840,7 +1844,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -1848,7 +1852,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -1856,7 +1860,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>132</v>
       </c>
@@ -1864,7 +1868,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>134</v>
       </c>
@@ -1872,7 +1876,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -1888,7 +1892,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -1896,7 +1900,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>142</v>
       </c>
@@ -1904,7 +1908,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -1912,7 +1916,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>146</v>
       </c>
@@ -1920,7 +1924,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>150</v>
       </c>
@@ -1936,7 +1940,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -1944,7 +1948,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>154</v>
       </c>
@@ -1952,7 +1956,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>156</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>160</v>
       </c>
@@ -1976,7 +1980,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -1992,7 +1996,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>166</v>
       </c>
@@ -2000,7 +2004,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>168</v>
       </c>
@@ -2008,7 +2012,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>170</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>172</v>
       </c>
@@ -2024,7 +2028,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>174</v>
       </c>
@@ -2032,7 +2036,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>176</v>
       </c>
@@ -2040,7 +2044,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>178</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>180</v>
       </c>
@@ -2056,7 +2060,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>182</v>
       </c>
@@ -2064,7 +2068,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>184</v>
       </c>
@@ -2072,7 +2076,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>186</v>
       </c>
@@ -2080,7 +2084,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -2088,7 +2092,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>190</v>
       </c>
@@ -2096,7 +2100,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>192</v>
       </c>
@@ -2104,7 +2108,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>194</v>
       </c>
@@ -2112,7 +2116,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>196</v>
       </c>
@@ -2120,7 +2124,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>198</v>
       </c>
@@ -2128,7 +2132,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>200</v>
       </c>
@@ -2136,7 +2140,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>202</v>
       </c>
@@ -2144,7 +2148,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>204</v>
       </c>
@@ -2152,7 +2156,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>206</v>
       </c>
@@ -2160,7 +2164,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>208</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>210</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>212</v>
       </c>
@@ -2184,7 +2188,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>214</v>
       </c>
@@ -2192,7 +2196,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>216</v>
       </c>
@@ -2200,7 +2204,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>218</v>
       </c>
@@ -2208,7 +2212,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>220</v>
       </c>
@@ -2216,7 +2220,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>222</v>
       </c>
@@ -2224,7 +2228,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>224</v>
       </c>
@@ -2232,7 +2236,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>226</v>
       </c>
@@ -2240,7 +2244,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>228</v>
       </c>
@@ -2248,7 +2252,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>230</v>
       </c>
@@ -2256,7 +2260,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>232</v>
       </c>
@@ -2264,7 +2268,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>234</v>
       </c>
@@ -2272,7 +2276,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>236</v>
       </c>
@@ -2280,7 +2284,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>238</v>
       </c>
@@ -2288,7 +2292,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>240</v>
       </c>
@@ -2296,7 +2300,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>242</v>
       </c>
@@ -2304,7 +2308,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>244</v>
       </c>
@@ -2312,7 +2316,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>246</v>
       </c>
@@ -2320,7 +2324,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>248</v>
       </c>
@@ -2328,7 +2332,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>250</v>
       </c>
@@ -2336,7 +2340,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>252</v>
       </c>
@@ -2344,7 +2348,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>254</v>
       </c>
@@ -2352,7 +2356,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>256</v>
       </c>
@@ -2360,7 +2364,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>258</v>
       </c>
@@ -2368,7 +2372,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>260</v>
       </c>
@@ -2376,7 +2380,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>262</v>
       </c>
@@ -2384,7 +2388,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>264</v>
       </c>
@@ -2392,7 +2396,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>266</v>
       </c>
@@ -2400,7 +2404,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>268</v>
       </c>
@@ -2408,7 +2412,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>270</v>
       </c>
@@ -2416,7 +2420,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>272</v>
       </c>
@@ -2424,7 +2428,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>274</v>
       </c>
@@ -2432,7 +2436,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>276</v>
       </c>
@@ -2440,7 +2444,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="b">
         <v>1</v>
       </c>
@@ -2448,7 +2452,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>279</v>
       </c>
@@ -2456,7 +2460,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>281</v>
       </c>
@@ -2464,7 +2468,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>283</v>
       </c>
@@ -2472,7 +2476,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>285</v>
       </c>
@@ -2480,7 +2484,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>287</v>
       </c>
@@ -2488,7 +2492,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>289</v>
       </c>
@@ -2496,7 +2500,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>291</v>
       </c>
@@ -2504,7 +2508,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>293</v>
       </c>
@@ -2512,7 +2516,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>295</v>
       </c>
@@ -2520,7 +2524,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>297</v>
       </c>
@@ -2528,7 +2532,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>299</v>
       </c>
@@ -2536,7 +2540,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>301</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>303</v>
       </c>
@@ -2552,7 +2556,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>305</v>
       </c>
@@ -2560,7 +2564,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>307</v>
       </c>
@@ -2568,7 +2572,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>309</v>
       </c>

</xml_diff>